<commit_message>
added 8/5 oct avoidance data
</commit_message>
<xml_diff>
--- a/octanol-avoidance.xlsx
+++ b/octanol-avoidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friv\git\cest-2.1-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mo555/git/projects/cest-2.1-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E400EDF9-EA37-4D9C-BBD1-35F9C0A7D517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8650AFF1-6941-2043-AA15-5F54EB379EE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A21FF16D-724C-444E-9619-C67945F33991}"/>
+    <workbookView xWindow="41880" yWindow="-5400" windowWidth="23440" windowHeight="14540" xr2:uid="{A21FF16D-724C-444E-9619-C67945F33991}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,19 +34,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="9">
   <si>
     <t>genotype</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>30pct_oct</t>
+  </si>
+  <si>
+    <t>odor</t>
+  </si>
+  <si>
+    <t>response.time</t>
+  </si>
+  <si>
+    <t>experimenter</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>cest-2.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,20 +418,869 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B428B1-7A7A-446F-8EA5-8D38C71AC507}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>2.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>3.2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3.2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2.7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>6.7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2.4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>7.3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>3.3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>7.7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1.5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>13.7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>6.2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>7.7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>5.5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>13.3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>1.6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>2.4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>1.5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>2.4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>3.1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>5.8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>1.9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>1.9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>1.8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>1.7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>4.7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>3.9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>4.3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>4.7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>1.7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>7.9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>2.1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>1.6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>1.6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>1.3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>3.3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>